<commit_message>
ASK-41 Correct reading lengths and section start / stop. Enable running all benchmarktests (not working fully)
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmartktest_traject 16-5.xlsx
+++ b/benchmarktests/testdefinitions/Benchmartktest_traject 16-5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6761D57C-5327-4E9A-849C-EF243BA7CB5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61869062-937F-4132-B448-3AFF2607D334}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="10" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="1" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -2208,7 +2208,7 @@
   </sheetPr>
   <dimension ref="B1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2909,14 +2909,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CBD9B7-2F4E-4E0F-B0DE-0C76068107FF}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2935,7 +2935,9 @@
       <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
       <c r="D3" s="52" t="s">
         <v>38</v>
       </c>
@@ -3144,7 +3146,7 @@
   <dimension ref="B2:Y32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3383,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="26">
-        <f t="shared" ref="H12:H13" si="6">G12*3.66</f>
+        <f t="shared" ref="H12" si="6">G12*3.66</f>
         <v>0</v>
       </c>
       <c r="I12" s="8" t="s">
@@ -3460,8 +3462,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="26">
-        <f t="shared" si="6"/>
-        <v>3.66</v>
+        <v>1</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>20</v>
@@ -4521,7 +4522,7 @@
   <dimension ref="B2:Y32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5298,8 +5299,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="26">
-        <f t="shared" si="9"/>
-        <v>2.3199999999999998</v>
+        <v>1</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>20</v>
@@ -5375,8 +5375,7 @@
         <v>0.5</v>
       </c>
       <c r="H20" s="26">
-        <f t="shared" si="9"/>
-        <v>1.1599999999999999</v>
+        <v>1</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
ASK-57 Include NotRelevant as an output option in the benchmarks
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmartktest_traject 16-5.xlsx
+++ b/benchmarktests/testdefinitions/Benchmartktest_traject 16-5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61869062-937F-4132-B448-3AFF2607D334}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E55E4D2-3BF5-4AD4-A29A-F6628B5D7055}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="1" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="10" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -2208,8 +2208,8 @@
   </sheetPr>
   <dimension ref="B1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,12 +2262,12 @@
         <v>2</v>
       </c>
       <c r="D3" s="22" t="str">
-        <f t="shared" ref="D3:D14" si="0">IF(COUNTIF(F3:L3,"D")&gt;0,"D",IF(COUNTIF(F3:L3,"-III")&gt;0,"-III",IF(COUNTIF(F3:L3,"-II")&gt;0,"-II",IF(COUNTIF(F3:L3,"-I")&gt;0,"-I",IF(COUNTIF(F3:L3,"+0")&gt;0,"+0",IF(COUNTIF(F3:L3,"+I")&gt;0,"+I",IF(COUNTIF(F3:L3,"+II")&gt;0,"+II",IF(COUNTIF(F3:L3,"+III")&gt;0,"+III","ND"))))))))</f>
-        <v>-I</v>
+        <f>IF(COUNTIF(F3:L3,"D")&gt;0,"D",IF(COUNTIF(F3:L3,"-III")&gt;0,"-III",IF(COUNTIF(F3:L3,"-II")&gt;0,"-II",IF(COUNTIF(F3:L3,"-I")&gt;0,"-I",IF(COUNTIF(F3:L3,"+0")&gt;0,"+0",IF(COUNTIF(F3:L3,"+I")&gt;0,"+I",IF(COUNTIF(F3:L3,"+II")&gt;0,"+II",IF(COUNTIF(F3:L3,"+III")&gt;0,"+III",IF(COUNTIF(F3:L3,"ND")&gt;0,"ND","NR")))))))))</f>
+        <v>+III</v>
       </c>
       <c r="E3" s="22" t="str">
-        <f t="shared" ref="E3:E14" si="1">IF(COUNTIF(F3:L3,"-III")&gt;0,"-III",IF(COUNTIF(F3:L3,"-II")&gt;0,"-II",IF(COUNTIF(F3:L3,"-I")&gt;0,"-I",IF(COUNTIF(F3:L3,"+0")&gt;0,"+0",IF(COUNTIF(F3:L3,"+I")&gt;0,"+I",IF(COUNTIF(F3:L3,"+II")&gt;0,"+II",IF(COUNTIF(F3:L3,"+III")&gt;0,"+III","ND")))))))</f>
-        <v>-I</v>
+        <f>IF(COUNTIF(F3:L3,"-III")&gt;0,"-III",IF(COUNTIF(F3:L3,"-II")&gt;0,"-II",IF(COUNTIF(F3:L3,"-I")&gt;0,"-I",IF(COUNTIF(F3:L3,"+0")&gt;0,"+0",IF(COUNTIF(F3:L3,"+I")&gt;0,"+I",IF(COUNTIF(F3:L3,"+II")&gt;0,"+II",IF(COUNTIF(F3:L3,"+III")&gt;0,"+III",IF(COUNTIF(F3:L3,"ND")&gt;0,"ND","NR"))))))))</f>
+        <v>+III</v>
       </c>
       <c r="F3" s="4" t="str">
         <f t="array" ref="F3">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B3,C3),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -2279,11 +2279,11 @@
       </c>
       <c r="H3" s="4" t="str">
         <f t="array" ref="H3">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B3,C3),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I3" s="4" t="str">
         <f t="array" ref="I3">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B3,C3),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J3" s="4" t="str">
         <f t="array" ref="J3">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B3,C3),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="K3" s="4" t="str">
         <f t="array" ref="K3">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B3,C3),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="L3" s="7" t="str">
         <f t="array" ref="L3">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B3,C3),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
@@ -2306,11 +2306,11 @@
         <v>4</v>
       </c>
       <c r="D4" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D4:D14" si="0">IF(COUNTIF(F4:L4,"D")&gt;0,"D",IF(COUNTIF(F4:L4,"-III")&gt;0,"-III",IF(COUNTIF(F4:L4,"-II")&gt;0,"-II",IF(COUNTIF(F4:L4,"-I")&gt;0,"-I",IF(COUNTIF(F4:L4,"+0")&gt;0,"+0",IF(COUNTIF(F4:L4,"+I")&gt;0,"+I",IF(COUNTIF(F4:L4,"+II")&gt;0,"+II",IF(COUNTIF(F4:L4,"+III")&gt;0,"+III",IF(COUNTIF(F4:L4,"ND")&gt;0,"ND","NR")))))))))</f>
         <v>-I</v>
       </c>
       <c r="E4" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E4:E14" si="1">IF(COUNTIF(F4:L4,"-III")&gt;0,"-III",IF(COUNTIF(F4:L4,"-II")&gt;0,"-II",IF(COUNTIF(F4:L4,"-I")&gt;0,"-I",IF(COUNTIF(F4:L4,"+0")&gt;0,"+0",IF(COUNTIF(F4:L4,"+I")&gt;0,"+I",IF(COUNTIF(F4:L4,"+II")&gt;0,"+II",IF(COUNTIF(F4:L4,"+III")&gt;0,"+III",IF(COUNTIF(F4:L4,"ND")&gt;0,"ND","NR"))))))))</f>
         <v>-I</v>
       </c>
       <c r="F4" s="9" t="str">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="H4" s="9" t="str">
         <f t="array" ref="H4">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B4,C4),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I4" s="9" t="str">
         <f t="array" ref="I4">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B4,C4),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J4" s="9" t="str">
         <f t="array" ref="J4">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B4,C4),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2367,11 +2367,11 @@
       </c>
       <c r="H5" s="9" t="str">
         <f t="array" ref="H5">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B5,C5),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I5" s="9" t="str">
         <f t="array" ref="I5">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B5,C5),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J5" s="9" t="str">
         <f t="array" ref="J5">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B5,C5),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2407,15 +2407,15 @@
       </c>
       <c r="G6" s="9" t="str">
         <f t="array" ref="G6">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B6,C6),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="H6" s="9" t="str">
         <f t="array" ref="H6">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B6,C6),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I6" s="9" t="str">
         <f t="array" ref="I6">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B6,C6),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J6" s="9" t="str">
         <f t="array" ref="J6">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B6,C6),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="L6" s="12" t="str">
         <f t="array" ref="L6">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B6,C6),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -2455,11 +2455,11 @@
       </c>
       <c r="H7" s="9" t="str">
         <f t="array" ref="H7">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B7,C7),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I7" s="9" t="str">
         <f t="array" ref="I7">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B7,C7),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J7" s="9" t="str">
         <f t="array" ref="J7">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B7,C7),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="L7" s="12" t="str">
         <f t="array" ref="L7">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B7,C7),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -2491,19 +2491,19 @@
       </c>
       <c r="F8" s="9" t="str">
         <f t="array" ref="F8">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B8,C8),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="G8" s="9" t="str">
         <f t="array" ref="G8">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B8,C8),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="H8" s="9" t="str">
         <f t="array" ref="H8">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B8,C8),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I8" s="9" t="str">
         <f t="array" ref="I8">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B8,C8),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J8" s="9" t="str">
         <f t="array" ref="J8">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B8,C8),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2511,7 +2511,7 @@
       </c>
       <c r="K8" s="9" t="str">
         <f t="array" ref="K8">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B8,C8),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="L8" s="12" t="str">
         <f t="array" ref="L8">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B8,C8),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="F9" s="9" t="str">
         <f t="array" ref="F9">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B9,C9),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="G9" s="9" t="str">
         <f t="array" ref="G9">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B9,C9),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
@@ -2543,11 +2543,11 @@
       </c>
       <c r="H9" s="9" t="str">
         <f t="array" ref="H9">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B9,C9),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I9" s="9" t="str">
         <f t="array" ref="I9">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B9,C9),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J9" s="9" t="str">
         <f t="array" ref="J9">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B9,C9),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="K9" s="9" t="str">
         <f t="array" ref="K9">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B9,C9),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="L9" s="12" t="str">
         <f t="array" ref="L9">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B9,C9),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="F10" s="9" t="str">
         <f t="array" ref="F10">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B10,C10),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="G10" s="9" t="str">
         <f t="array" ref="G10">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B10,C10),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
@@ -2587,11 +2587,11 @@
       </c>
       <c r="H10" s="9" t="str">
         <f t="array" ref="H10">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B10,C10),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I10" s="9" t="str">
         <f t="array" ref="I10">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B10,C10),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J10" s="9" t="str">
         <f t="array" ref="J10">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B10,C10),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2631,11 +2631,11 @@
       </c>
       <c r="H11" s="9" t="str">
         <f t="array" ref="H11">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B11,C11),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I11" s="9" t="str">
         <f t="array" ref="I11">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B11,C11),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J11" s="9" t="str">
         <f t="array" ref="J11">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B11,C11),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2675,11 +2675,11 @@
       </c>
       <c r="H12" s="9" t="str">
         <f t="array" ref="H12">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B12,C12),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I12" s="9" t="str">
         <f t="array" ref="I12">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B12,C12),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J12" s="9" t="str">
         <f t="array" ref="J12">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B12,C12),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2719,11 +2719,11 @@
       </c>
       <c r="H13" s="9" t="str">
         <f t="array" ref="H13">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B13,C13),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I13" s="9" t="str">
         <f t="array" ref="I13">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B13,C13),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J13" s="9" t="str">
         <f t="array" ref="J13">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B13,C13),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
@@ -2763,15 +2763,15 @@
       </c>
       <c r="H14" s="9" t="str">
         <f t="array" ref="H14">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B14,C14),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="I14" s="9" t="str">
         <f t="array" ref="I14">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B14,C14),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>NR</v>
       </c>
       <c r="J14" s="9" t="str">
         <f t="array" ref="J14">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B14,C14),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="K14" s="9" t="str">
         <f t="array" ref="K14">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B14,C14),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
@@ -2909,7 +2909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CBD9B7-2F4E-4E0F-B0DE-0C76068107FF}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3146,7 +3146,7 @@
   <dimension ref="B2:Y32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3329,11 +3329,11 @@
         <v>-</v>
       </c>
       <c r="O11" s="30" t="str">
-        <f t="shared" ref="O11:O22" si="3">IF(ISNUMBER($M11),W11,IF($X11,"D","ND"))</f>
+        <f>IF(E11="Nee","NR",IF(ISNUMBER($M11),W11,IF($X11,"D","ND")))</f>
         <v>ND</v>
       </c>
       <c r="Q11" s="31">
-        <f t="shared" ref="Q11:Q22" si="4">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
+        <f t="shared" ref="Q11:Q22" si="3">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
         <v>1</v>
       </c>
       <c r="R11" s="10">
@@ -3341,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="S11" s="10">
-        <f t="shared" ref="S11:S22" si="5">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
+        <f t="shared" ref="S11:S22" si="4">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="T11" s="10">
@@ -3385,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="26">
-        <f t="shared" ref="H12" si="6">G12*3.66</f>
+        <f t="shared" ref="H12" si="5">G12*3.66</f>
         <v>0</v>
       </c>
       <c r="I12" s="8" t="s">
@@ -3406,11 +3406,11 @@
         <v>1</v>
       </c>
       <c r="O12" s="32" t="str">
+        <f t="shared" ref="O11:O22" si="6">IF(E12="Nee","NR",IF(ISNUMBER($M12),W12,IF($X12,"D","ND")))</f>
+        <v>+III</v>
+      </c>
+      <c r="Q12" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q12" s="31">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R12" s="10">
@@ -3418,7 +3418,7 @@
         <v>1</v>
       </c>
       <c r="S12" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T12" s="10">
@@ -3486,11 +3486,11 @@
         <v>1</v>
       </c>
       <c r="O13" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>+III</v>
+      </c>
+      <c r="Q13" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q13" s="31">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R13" s="10">
@@ -3498,7 +3498,7 @@
         <v>1</v>
       </c>
       <c r="S13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T13" s="10">
@@ -3563,11 +3563,11 @@
         <v>-</v>
       </c>
       <c r="O14" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>D</v>
+      </c>
+      <c r="Q14" s="31" t="e">
         <f t="shared" si="3"/>
-        <v>D</v>
-      </c>
-      <c r="Q14" s="31" t="e">
-        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="R14" s="10">
@@ -3575,7 +3575,7 @@
         <v>1</v>
       </c>
       <c r="S14" s="10" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="T14" s="10">
@@ -3643,11 +3643,11 @@
         <v>3.6599999999999997</v>
       </c>
       <c r="O15" s="32" t="str">
+        <f t="shared" si="6"/>
+        <v>-I</v>
+      </c>
+      <c r="Q15" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q15" s="31">
-        <f t="shared" si="4"/>
         <v>0.99998169999999997</v>
       </c>
       <c r="R15" s="10">
@@ -3655,7 +3655,7 @@
         <v>0.99998169999999997</v>
       </c>
       <c r="S15" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4450000000000002E-4</v>
       </c>
       <c r="T15" s="10">
@@ -3715,11 +3715,11 @@
         <v>1</v>
       </c>
       <c r="O16" s="32" t="str">
+        <f>IF(E16="Nee","NR",IF(ISNUMBER($M16),W16,IF($X16,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="Q16" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q16" s="31">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R16" s="10">
@@ -3727,7 +3727,7 @@
         <v>1</v>
       </c>
       <c r="S16" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T16" s="10">
@@ -3787,11 +3787,11 @@
         <v>1</v>
       </c>
       <c r="O17" s="32" t="str">
+        <f t="shared" ref="O17:O22" si="10">IF(E17="Nee","NR",IF(ISNUMBER($M17),W17,IF($X17,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="Q17" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q17" s="31">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R17" s="10">
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="S17" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T17" s="10">
@@ -3859,11 +3859,11 @@
         <v>1</v>
       </c>
       <c r="O18" s="32" t="str">
+        <f t="shared" si="10"/>
+        <v>NR</v>
+      </c>
+      <c r="Q18" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q18" s="31">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R18" s="10">
@@ -3871,7 +3871,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T18" s="10">
@@ -3915,7 +3915,7 @@
         <v>7.27E-4</v>
       </c>
       <c r="H19" s="26">
-        <f t="shared" ref="H19:H22" si="10">G19*3.66</f>
+        <f t="shared" ref="H19:H22" si="11">G19*3.66</f>
         <v>2.6608199999999999E-3</v>
       </c>
       <c r="I19" s="8" t="s">
@@ -3936,11 +3936,11 @@
         <v>3.66</v>
       </c>
       <c r="O19" s="32" t="str">
+        <f t="shared" si="10"/>
+        <v>-I</v>
+      </c>
+      <c r="Q19" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q19" s="31">
-        <f t="shared" si="4"/>
         <v>0.99733917999999999</v>
       </c>
       <c r="R19" s="10">
@@ -3948,7 +3948,7 @@
         <v>0.99733917999999999</v>
       </c>
       <c r="S19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.1010299999999999E-2</v>
       </c>
       <c r="T19" s="10">
@@ -3992,7 +3992,7 @@
         <v>7.2800000000000002E-4</v>
       </c>
       <c r="H20" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.6644800000000003E-3</v>
       </c>
       <c r="I20" s="8" t="s">
@@ -4017,11 +4017,11 @@
         <v>1</v>
       </c>
       <c r="O20" s="32" t="str">
+        <f t="shared" si="10"/>
+        <v>+III</v>
+      </c>
+      <c r="Q20" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q20" s="31">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R20" s="10">
@@ -4029,7 +4029,7 @@
         <v>1</v>
       </c>
       <c r="S20" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T20" s="10">
@@ -4073,7 +4073,7 @@
         <v>1E-10</v>
       </c>
       <c r="H21" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.6600000000000003E-10</v>
       </c>
       <c r="I21" s="8" t="s">
@@ -4094,11 +4094,11 @@
         <v>3.66</v>
       </c>
       <c r="O21" s="32" t="str">
+        <f t="shared" si="10"/>
+        <v>-I</v>
+      </c>
+      <c r="Q21" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q21" s="31">
-        <f t="shared" si="4"/>
         <v>0.99999999963399999</v>
       </c>
       <c r="R21" s="10">
@@ -4106,7 +4106,7 @@
         <v>0.99999999963399999</v>
       </c>
       <c r="S21" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.8900000000000002E-9</v>
       </c>
       <c r="T21" s="10">
@@ -4150,7 +4150,7 @@
         <v>1E-4</v>
       </c>
       <c r="H22" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.6600000000000001E-4</v>
       </c>
       <c r="I22" s="8" t="s">
@@ -4171,11 +4171,11 @@
         <v>3.6599999999999997</v>
       </c>
       <c r="O22" s="32" t="str">
+        <f t="shared" si="10"/>
+        <v>-I</v>
+      </c>
+      <c r="Q22" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q22" s="31">
-        <f t="shared" si="4"/>
         <v>0.99963400000000002</v>
       </c>
       <c r="R22" s="10">
@@ -4183,7 +4183,7 @@
         <v>0.99963400000000002</v>
       </c>
       <c r="S22" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.8900000000000002E-3</v>
       </c>
       <c r="T22" s="10">
@@ -4504,7 +4504,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E7586F0-4A97-4FE3-A954-2F42494980C3}">
           <x14:formula1>
             <xm:f>Informatiepagina!$B$15:$B$17</xm:f>
@@ -4522,7 +4522,7 @@
   <dimension ref="B2:Y32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4709,11 +4709,11 @@
         <v>1</v>
       </c>
       <c r="O11" s="30" t="str">
-        <f t="shared" ref="O11:O22" si="3">IF(ISNUMBER($M11),W11,IF($X11,"D","ND"))</f>
+        <f>IF(E11="Nee","NR",IF(ISNUMBER($M11),W11,IF($X11,"D","ND")))</f>
         <v>+III</v>
       </c>
       <c r="Q11" s="31">
-        <f t="shared" ref="Q11:Q22" si="4">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
+        <f t="shared" ref="Q11:Q22" si="3">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
         <v>1</v>
       </c>
       <c r="R11" s="10">
@@ -4721,7 +4721,7 @@
         <v>1</v>
       </c>
       <c r="S11" s="10">
-        <f t="shared" ref="S11:S22" si="5">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
+        <f t="shared" ref="S11:S22" si="4">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="T11" s="10">
@@ -4785,23 +4785,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O12" s="32" t="str">
+        <f>IF(E12="Nee","NR",IF(ISNUMBER($M12),W12,IF($X12,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="Q12" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q12" s="31">
+        <v>0.99945015999999998</v>
+      </c>
+      <c r="R12" s="10">
+        <f t="shared" ref="R12:R22" si="5">IF(M12="-",1,Q12)</f>
+        <v>0.99945015999999998</v>
+      </c>
+      <c r="S12" s="10">
         <f t="shared" si="4"/>
-        <v>0.99945015999999998</v>
-      </c>
-      <c r="R12" s="10">
-        <f t="shared" ref="R12:R22" si="6">IF(M12="-",1,Q12)</f>
-        <v>0.99945015999999998</v>
-      </c>
-      <c r="S12" s="10">
-        <f t="shared" si="5"/>
         <v>3.5076E-3</v>
       </c>
       <c r="T12" s="10">
-        <f t="shared" ref="T12:T22" si="7">IF(L12="-",0,S12)</f>
+        <f t="shared" ref="T12:T22" si="6">IF(L12="-",0,S12)</f>
         <v>3.5076E-3</v>
       </c>
       <c r="U12" s="9">
@@ -4817,7 +4817,7 @@
         <v>-I</v>
       </c>
       <c r="X12" s="12" t="b">
-        <f t="shared" ref="X12:X22" si="8">IF($E12="Ja",IF($I12="Ja",NOT(ISNUMBER($J12)),FALSE),FALSE)</f>
+        <f t="shared" ref="X12:X22" si="7">IF($E12="Ja",IF($I12="Ja",NOT(ISNUMBER($J12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -4861,23 +4861,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O13" s="32" t="str">
+        <f>IF(E13="Nee","NR",IF(ISNUMBER($M13),W13,IF($X13,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="Q13" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q13" s="31">
+        <v>1</v>
+      </c>
+      <c r="R13" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S13" s="10">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="R13" s="10">
+        <v>1.48E-49</v>
+      </c>
+      <c r="T13" s="10">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S13" s="10">
-        <f t="shared" si="5"/>
-        <v>1.48E-49</v>
-      </c>
-      <c r="T13" s="10">
-        <f t="shared" si="7"/>
         <v>1.48E-49</v>
       </c>
       <c r="U13" s="9">
@@ -4893,7 +4893,7 @@
         <v>-I</v>
       </c>
       <c r="X13" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4933,23 +4933,23 @@
         <v>1</v>
       </c>
       <c r="O14" s="32" t="str">
+        <f>IF(E14="Nee","NR",IF(ISNUMBER($M14),W14,IF($X14,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="Q14" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q14" s="31">
+        <v>1</v>
+      </c>
+      <c r="R14" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S14" s="10">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="R14" s="10">
+        <v>0</v>
+      </c>
+      <c r="T14" s="10">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S14" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="10">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U14" s="9">
@@ -4965,7 +4965,7 @@
         <v>+III</v>
       </c>
       <c r="X14" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5009,23 +5009,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O15" s="32" t="str">
+        <f>IF(E15="Nee","NR",IF(ISNUMBER($M15),W15,IF($X15,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="Q15" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q15" s="31">
+        <v>0.99944895359999997</v>
+      </c>
+      <c r="R15" s="10">
+        <f t="shared" si="5"/>
+        <v>0.99944895359999997</v>
+      </c>
+      <c r="S15" s="10">
         <f t="shared" si="4"/>
-        <v>0.99944895359999997</v>
-      </c>
-      <c r="R15" s="10">
+        <v>3.5152960000000002E-3</v>
+      </c>
+      <c r="T15" s="10">
         <f t="shared" si="6"/>
-        <v>0.99944895359999997</v>
-      </c>
-      <c r="S15" s="10">
-        <f t="shared" si="5"/>
-        <v>3.5152960000000002E-3</v>
-      </c>
-      <c r="T15" s="10">
-        <f t="shared" si="7"/>
         <v>3.5152960000000002E-3</v>
       </c>
       <c r="U15" s="9">
@@ -5041,7 +5041,7 @@
         <v>-I</v>
       </c>
       <c r="X15" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5081,23 +5081,23 @@
         <v>1</v>
       </c>
       <c r="O16" s="32" t="str">
+        <f>IF(E16="Nee","NR",IF(ISNUMBER($M16),W16,IF($X16,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="Q16" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q16" s="31">
+        <v>1</v>
+      </c>
+      <c r="R16" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S16" s="10">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="R16" s="10">
+        <v>0</v>
+      </c>
+      <c r="T16" s="10">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S16" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T16" s="10">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U16" s="9">
@@ -5113,7 +5113,7 @@
         <v>+III</v>
       </c>
       <c r="X16" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5162,23 +5162,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O17" s="32" t="str">
+        <f>IF(E17="Nee","NR",IF(ISNUMBER($M17),W17,IF($X17,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="Q17" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q17" s="31">
+        <v>0.9999768</v>
+      </c>
+      <c r="R17" s="10">
+        <f t="shared" si="5"/>
+        <v>0.9999768</v>
+      </c>
+      <c r="S17" s="10">
         <f t="shared" si="4"/>
-        <v>0.9999768</v>
-      </c>
-      <c r="R17" s="10">
+        <v>1.4800000000000002E-4</v>
+      </c>
+      <c r="T17" s="10">
         <f t="shared" si="6"/>
-        <v>0.9999768</v>
-      </c>
-      <c r="S17" s="10">
-        <f t="shared" si="5"/>
-        <v>1.4800000000000002E-4</v>
-      </c>
-      <c r="T17" s="10">
-        <f t="shared" si="7"/>
         <v>1.4800000000000002E-4</v>
       </c>
       <c r="U17" s="9">
@@ -5194,7 +5194,7 @@
         <v>-I</v>
       </c>
       <c r="X17" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5218,7 +5218,7 @@
         <v>2.3800000000000001E-4</v>
       </c>
       <c r="H18" s="26">
-        <f t="shared" ref="H18:H22" si="9">G18*2.32</f>
+        <f t="shared" ref="H18:H22" si="8">G18*2.32</f>
         <v>5.5216E-4</v>
       </c>
       <c r="I18" s="8" t="s">
@@ -5243,23 +5243,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O18" s="32" t="str">
+        <f>IF(E18="Nee","NR",IF(ISNUMBER($M18),W18,IF($X18,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="Q18" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q18" s="31">
+        <v>0.99999999976800003</v>
+      </c>
+      <c r="R18" s="10">
+        <f t="shared" si="5"/>
+        <v>0.99999999976800003</v>
+      </c>
+      <c r="S18" s="10">
         <f t="shared" si="4"/>
-        <v>0.99999999976800003</v>
-      </c>
-      <c r="R18" s="10">
+        <v>1.4800000000000001E-9</v>
+      </c>
+      <c r="T18" s="10">
         <f t="shared" si="6"/>
-        <v>0.99999999976800003</v>
-      </c>
-      <c r="S18" s="10">
-        <f t="shared" si="5"/>
-        <v>1.4800000000000001E-9</v>
-      </c>
-      <c r="T18" s="10">
-        <f t="shared" si="7"/>
         <v>1.4800000000000001E-9</v>
       </c>
       <c r="U18" s="9">
@@ -5275,7 +5275,7 @@
         <v>-I</v>
       </c>
       <c r="X18" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5319,23 +5319,23 @@
         <v>-</v>
       </c>
       <c r="O19" s="32" t="str">
+        <f>IF(E19="Nee","NR",IF(ISNUMBER($M19),W19,IF($X19,"D","ND")))</f>
+        <v>D</v>
+      </c>
+      <c r="Q19" s="31" t="e">
         <f t="shared" si="3"/>
-        <v>D</v>
-      </c>
-      <c r="Q19" s="31" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R19" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S19" s="10" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="R19" s="10">
+      <c r="T19" s="10">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S19" s="10" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T19" s="10">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U19" s="9">
@@ -5351,7 +5351,7 @@
         <v>+III</v>
       </c>
       <c r="X19" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5387,11 +5387,11 @@
         <v>0</v>
       </c>
       <c r="L20" s="31">
-        <f t="shared" ref="L20:L22" si="10">IF($E20="Nee",0,IF(I20="Ja",IF(ISNUMBER(J20),J20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
+        <f t="shared" ref="L20:L22" si="9">IF($E20="Nee",0,IF(I20="Ja",IF(ISNUMBER(J20),J20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
         <v>0</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" ref="M20:M22" si="11">IF($E20="Nee",0,IF(I20="Ja",IF(ISNUMBER(K20),K20,"-"),IF(ISNUMBER(H20),H20,"-")))</f>
+        <f t="shared" ref="M20:M22" si="10">IF($E20="Nee",0,IF(I20="Ja",IF(ISNUMBER(K20),K20,"-"),IF(ISNUMBER(H20),H20,"-")))</f>
         <v>0</v>
       </c>
       <c r="N20" s="11">
@@ -5399,23 +5399,23 @@
         <v>1</v>
       </c>
       <c r="O20" s="32" t="str">
+        <f>IF(E20="Nee","NR",IF(ISNUMBER($M20),W20,IF($X20,"D","ND")))</f>
+        <v>+III</v>
+      </c>
+      <c r="Q20" s="31">
         <f t="shared" si="3"/>
-        <v>+III</v>
-      </c>
-      <c r="Q20" s="31">
+        <v>1</v>
+      </c>
+      <c r="R20" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S20" s="10">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="R20" s="10">
+        <v>0</v>
+      </c>
+      <c r="T20" s="10">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S20" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="10">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U20" s="9">
@@ -5431,7 +5431,7 @@
         <v>+III</v>
       </c>
       <c r="X20" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5455,7 +5455,7 @@
         <v>0.1</v>
       </c>
       <c r="H21" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.23199999999999998</v>
       </c>
       <c r="I21" s="8" t="s">
@@ -5468,11 +5468,11 @@
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="L21" s="31">
+        <f t="shared" si="9"/>
+        <v>1E-8</v>
+      </c>
+      <c r="M21" s="10">
         <f t="shared" si="10"/>
-        <v>1E-8</v>
-      </c>
-      <c r="M21" s="10">
-        <f t="shared" si="11"/>
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="N21" s="11">
@@ -5480,23 +5480,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O21" s="32" t="str">
+        <f>IF(E21="Nee","NR",IF(ISNUMBER($M21),W21,IF($X21,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="Q21" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q21" s="31">
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="R21" s="10">
+        <f t="shared" si="5"/>
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="S21" s="10">
         <f t="shared" si="4"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="R21" s="10">
+        <v>1.48E-7</v>
+      </c>
+      <c r="T21" s="10">
         <f t="shared" si="6"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="S21" s="10">
-        <f t="shared" si="5"/>
-        <v>1.48E-7</v>
-      </c>
-      <c r="T21" s="10">
-        <f t="shared" si="7"/>
         <v>1.48E-7</v>
       </c>
       <c r="U21" s="9">
@@ -5512,7 +5512,7 @@
         <v>-I</v>
       </c>
       <c r="X21" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5536,7 +5536,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="H22" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.22968</v>
       </c>
       <c r="I22" s="8" t="s">
@@ -5549,11 +5549,11 @@
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="L22" s="31">
+        <f t="shared" si="9"/>
+        <v>1E-8</v>
+      </c>
+      <c r="M22" s="10">
         <f t="shared" si="10"/>
-        <v>1E-8</v>
-      </c>
-      <c r="M22" s="10">
-        <f t="shared" si="11"/>
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="N22" s="11">
@@ -5561,23 +5561,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O22" s="32" t="str">
+        <f>IF(E22="Nee","NR",IF(ISNUMBER($M22),W22,IF($X22,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="Q22" s="31">
         <f t="shared" si="3"/>
-        <v>-I</v>
-      </c>
-      <c r="Q22" s="31">
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="R22" s="10">
+        <f t="shared" si="5"/>
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="S22" s="10">
         <f t="shared" si="4"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="R22" s="10">
+        <v>1.48E-7</v>
+      </c>
+      <c r="T22" s="10">
         <f t="shared" si="6"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="S22" s="10">
-        <f t="shared" si="5"/>
-        <v>1.48E-7</v>
-      </c>
-      <c r="T22" s="10">
-        <f t="shared" si="7"/>
         <v>1.48E-7</v>
       </c>
       <c r="U22" s="9">
@@ -5593,7 +5593,7 @@
         <v>-I</v>
       </c>
       <c r="X22" s="12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5912,7 +5912,7 @@
   <dimension ref="B2:U73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6069,19 +6069,19 @@
         <v>0</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f t="shared" ref="K11" si="0">IF(ISNUMBER($J11),S11,IF($T11,"D","ND"))</f>
-        <v>-I</v>
+        <f>IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
+        <v>NR</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" ref="M11" si="1">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11" si="0">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>1</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11" si="2">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11" si="1">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11" si="3">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
+        <f t="shared" ref="O11" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P11" s="10">
@@ -7428,7 +7428,7 @@
   <dimension ref="B2:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7585,8 +7585,8 @@
         <v>0</v>
       </c>
       <c r="K11" s="47" t="str">
-        <f>IF(ISNUMBER($J11),S11,IF($T11,"D","ND"))</f>
-        <v>-I</v>
+        <f>IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
+        <v>NR</v>
       </c>
       <c r="M11" s="33">
         <f>IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
@@ -7750,7 +7750,7 @@
   <dimension ref="B2:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="K11" sqref="K11:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7907,19 +7907,19 @@
         <v>-</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f t="shared" ref="K11:K12" si="1">IF(ISNUMBER($J11),S11,IF($T11,"D","ND"))</f>
+        <f>IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
         <v>ND</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" ref="M11:M12" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11:M12" si="1">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>1</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N12" si="3">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11:N12" si="2">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11:O12" si="4">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
+        <f t="shared" ref="O11:O12" si="3">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P11" s="10">
@@ -7973,23 +7973,23 @@
         <v>0</v>
       </c>
       <c r="K12" s="32" t="str">
+        <f>IF($E12="Nee","NR",IF(ISNUMBER($J12),S12,IF($T12,"D","ND")))</f>
+        <v>+III</v>
+      </c>
+      <c r="M12" s="31">
         <f t="shared" si="1"/>
-        <v>+III</v>
-      </c>
-      <c r="M12" s="31">
+        <v>1</v>
+      </c>
+      <c r="N12" s="10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N12" s="10">
+      <c r="O12" s="10">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="10">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P13" si="5">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P13" si="4">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
@@ -8005,7 +8005,7 @@
         <v>+III</v>
       </c>
       <c r="T12" s="12" t="b">
-        <f t="shared" ref="T12:T22" si="6">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="5">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -8039,23 +8039,23 @@
         <v>5.9999999999999997E-7</v>
       </c>
       <c r="K13" s="32" t="str">
-        <f t="shared" ref="K13:K22" si="7">IF(ISNUMBER($J13),S13,IF($T13,"D","ND"))</f>
+        <f>IF($E13="Nee","NR",IF(ISNUMBER($J13),S13,IF($T13,"D","ND")))</f>
         <v>-I</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" ref="M13:M22" si="8">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
+        <f t="shared" ref="M13:M22" si="6">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
         <v>0.99999939999999998</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" ref="N13:N22" si="9">IF(J13="-",1,M13)</f>
+        <f t="shared" ref="N13:N22" si="7">IF(J13="-",1,M13)</f>
         <v>0.99999939999999998</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" ref="O13:O22" si="10">IF(AND(F13="Geen faalkans",H13="Nee"),0,J13*$C$3)</f>
+        <f t="shared" ref="O13:O22" si="8">IF(AND(F13="Geen faalkans",H13="Nee"),0,J13*$C$3)</f>
         <v>1.7999999999999999E-6</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.7999999999999999E-6</v>
       </c>
       <c r="Q13" s="9">
@@ -8071,7 +8071,7 @@
         <v>-I</v>
       </c>
       <c r="T13" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8103,23 +8103,23 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="K14" s="32" t="str">
+        <f>IF($E14="Nee","NR",IF(ISNUMBER($J14),S14,IF($T14,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M14" s="31">
+        <f t="shared" si="6"/>
+        <v>0.99999499999999997</v>
+      </c>
+      <c r="N14" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M14" s="31">
+        <v>0.99999499999999997</v>
+      </c>
+      <c r="O14" s="10">
         <f t="shared" si="8"/>
-        <v>0.99999499999999997</v>
-      </c>
-      <c r="N14" s="10">
-        <f t="shared" si="9"/>
-        <v>0.99999499999999997</v>
-      </c>
-      <c r="O14" s="10">
-        <f t="shared" si="10"/>
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" ref="P14:P22" si="11">IF(J14="-",0,O14)</f>
+        <f t="shared" ref="P14:P22" si="9">IF(J14="-",0,O14)</f>
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="Q14" s="9">
@@ -8135,7 +8135,7 @@
         <v>-I</v>
       </c>
       <c r="T14" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8169,23 +8169,23 @@
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="K15" s="32" t="str">
+        <f>IF($E15="Nee","NR",IF(ISNUMBER($J15),S15,IF($T15,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M15" s="31">
+        <f t="shared" si="6"/>
+        <v>0.999999992</v>
+      </c>
+      <c r="N15" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M15" s="31">
+        <v>0.999999992</v>
+      </c>
+      <c r="O15" s="10">
         <f t="shared" si="8"/>
-        <v>0.999999992</v>
-      </c>
-      <c r="N15" s="10">
+        <v>2.4000000000000003E-8</v>
+      </c>
+      <c r="P15" s="10">
         <f t="shared" si="9"/>
-        <v>0.999999992</v>
-      </c>
-      <c r="O15" s="10">
-        <f t="shared" si="10"/>
-        <v>2.4000000000000003E-8</v>
-      </c>
-      <c r="P15" s="10">
-        <f t="shared" si="11"/>
         <v>2.4000000000000003E-8</v>
       </c>
       <c r="Q15" s="9">
@@ -8201,7 +8201,7 @@
         <v>-I</v>
       </c>
       <c r="T15" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8235,23 +8235,23 @@
         <v>0</v>
       </c>
       <c r="K16" s="32" t="str">
+        <f>IF($E16="Nee","NR",IF(ISNUMBER($J16),S16,IF($T16,"D","ND")))</f>
+        <v>+III</v>
+      </c>
+      <c r="M16" s="31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N16" s="10">
         <f t="shared" si="7"/>
-        <v>+III</v>
-      </c>
-      <c r="M16" s="31">
+        <v>1</v>
+      </c>
+      <c r="O16" s="10">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N16" s="10">
+        <v>0</v>
+      </c>
+      <c r="P16" s="10">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="O16" s="10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="10">
-        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q16" s="9">
@@ -8267,7 +8267,7 @@
         <v>+III</v>
       </c>
       <c r="T16" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8301,23 +8301,23 @@
         <v>2.546E-5</v>
       </c>
       <c r="K17" s="32" t="str">
+        <f>IF($E17="Nee","NR",IF(ISNUMBER($J17),S17,IF($T17,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M17" s="31">
+        <f t="shared" si="6"/>
+        <v>0.99997453999999997</v>
+      </c>
+      <c r="N17" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M17" s="31">
+        <v>0.99997453999999997</v>
+      </c>
+      <c r="O17" s="10">
         <f t="shared" si="8"/>
-        <v>0.99997453999999997</v>
-      </c>
-      <c r="N17" s="10">
+        <v>7.6379999999999997E-5</v>
+      </c>
+      <c r="P17" s="10">
         <f t="shared" si="9"/>
-        <v>0.99997453999999997</v>
-      </c>
-      <c r="O17" s="10">
-        <f t="shared" si="10"/>
-        <v>7.6379999999999997E-5</v>
-      </c>
-      <c r="P17" s="10">
-        <f t="shared" si="11"/>
         <v>7.6379999999999997E-5</v>
       </c>
       <c r="Q17" s="9">
@@ -8333,7 +8333,7 @@
         <v>-I</v>
       </c>
       <c r="T17" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8365,23 +8365,23 @@
         <v>6.6600000000000003E-4</v>
       </c>
       <c r="K18" s="32" t="str">
+        <f>IF($E18="Nee","NR",IF(ISNUMBER($J18),S18,IF($T18,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M18" s="31">
+        <f t="shared" si="6"/>
+        <v>0.99933399999999994</v>
+      </c>
+      <c r="N18" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M18" s="31">
+        <v>0.99933399999999994</v>
+      </c>
+      <c r="O18" s="10">
         <f t="shared" si="8"/>
-        <v>0.99933399999999994</v>
-      </c>
-      <c r="N18" s="10">
+        <v>1.9980000000000002E-3</v>
+      </c>
+      <c r="P18" s="10">
         <f t="shared" si="9"/>
-        <v>0.99933399999999994</v>
-      </c>
-      <c r="O18" s="10">
-        <f t="shared" si="10"/>
-        <v>1.9980000000000002E-3</v>
-      </c>
-      <c r="P18" s="10">
-        <f t="shared" si="11"/>
         <v>1.9980000000000002E-3</v>
       </c>
       <c r="Q18" s="9">
@@ -8397,7 +8397,7 @@
         <v>-I</v>
       </c>
       <c r="T18" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8431,23 +8431,23 @@
         <v>1.2999999999999999E-3</v>
       </c>
       <c r="K19" s="32" t="str">
+        <f>IF($E19="Nee","NR",IF(ISNUMBER($J19),S19,IF($T19,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M19" s="31">
+        <f t="shared" si="6"/>
+        <v>0.99870000000000003</v>
+      </c>
+      <c r="N19" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M19" s="31">
+        <v>0.99870000000000003</v>
+      </c>
+      <c r="O19" s="10">
         <f t="shared" si="8"/>
-        <v>0.99870000000000003</v>
-      </c>
-      <c r="N19" s="10">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="P19" s="10">
         <f t="shared" si="9"/>
-        <v>0.99870000000000003</v>
-      </c>
-      <c r="O19" s="10">
-        <f t="shared" si="10"/>
-        <v>3.8999999999999998E-3</v>
-      </c>
-      <c r="P19" s="10">
-        <f t="shared" si="11"/>
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="Q19" s="9">
@@ -8463,7 +8463,7 @@
         <v>-I</v>
       </c>
       <c r="T19" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8495,23 +8495,23 @@
         <v>0</v>
       </c>
       <c r="K20" s="32" t="str">
+        <f>IF($E20="Nee","NR",IF(ISNUMBER($J20),S20,IF($T20,"D","ND")))</f>
+        <v>+III</v>
+      </c>
+      <c r="M20" s="31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N20" s="10">
         <f t="shared" si="7"/>
-        <v>+III</v>
-      </c>
-      <c r="M20" s="31">
+        <v>1</v>
+      </c>
+      <c r="O20" s="10">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N20" s="10">
+        <v>0</v>
+      </c>
+      <c r="P20" s="10">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="10">
-        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q20" s="9">
@@ -8527,7 +8527,7 @@
         <v>+III</v>
       </c>
       <c r="T20" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8561,23 +8561,23 @@
         <v>0</v>
       </c>
       <c r="K21" s="32" t="str">
+        <f>IF($E21="Nee","NR",IF(ISNUMBER($J21),S21,IF($T21,"D","ND")))</f>
+        <v>+III</v>
+      </c>
+      <c r="M21" s="31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N21" s="10">
         <f t="shared" si="7"/>
-        <v>+III</v>
-      </c>
-      <c r="M21" s="31">
+        <v>1</v>
+      </c>
+      <c r="O21" s="10">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N21" s="10">
+        <v>0</v>
+      </c>
+      <c r="P21" s="10">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="O21" s="10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="10">
-        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q21" s="9">
@@ -8593,7 +8593,7 @@
         <v>+III</v>
       </c>
       <c r="T21" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8623,23 +8623,23 @@
         <v>0</v>
       </c>
       <c r="K22" s="32" t="str">
+        <f>IF($E22="Nee","NR",IF(ISNUMBER($J22),S22,IF($T22,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="M22" s="31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N22" s="10">
         <f t="shared" si="7"/>
-        <v>+III</v>
-      </c>
-      <c r="M22" s="31">
+        <v>1</v>
+      </c>
+      <c r="O22" s="10">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N22" s="10">
+        <v>0</v>
+      </c>
+      <c r="P22" s="10">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="O22" s="10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="10">
-        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q22" s="9">
@@ -8655,7 +8655,7 @@
         <v>+III</v>
       </c>
       <c r="T22" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8902,7 +8902,7 @@
   <dimension ref="B2:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="K11" sqref="K11:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9059,19 +9059,19 @@
         <v>0</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f t="shared" ref="K11:K22" si="1">IF(ISNUMBER($J11),S11,IF($T11,"D","ND"))</f>
-        <v>-I</v>
+        <f>IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
+        <v>NR</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" ref="M11:M22" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11:M22" si="1">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>1</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N22" si="3">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11:N22" si="2">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11:O22" si="4">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
+        <f t="shared" ref="O11:O22" si="3">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P11" s="10">
@@ -9121,23 +9121,23 @@
         <v>-</v>
       </c>
       <c r="K12" s="32" t="str">
+        <f>IF($E12="Nee","NR",IF(ISNUMBER($J12),S12,IF($T12,"D","ND")))</f>
+        <v>ND</v>
+      </c>
+      <c r="M12" s="31">
         <f t="shared" si="1"/>
-        <v>ND</v>
-      </c>
-      <c r="M12" s="31">
+        <v>1</v>
+      </c>
+      <c r="N12" s="10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N12" s="10">
+      <c r="O12" s="10">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="10">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P22" si="5">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P22" si="4">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
@@ -9153,7 +9153,7 @@
         <v>+0</v>
       </c>
       <c r="T12" s="12" t="b">
-        <f t="shared" ref="T12:T22" si="6">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="5">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -9187,23 +9187,23 @@
         <v>0</v>
       </c>
       <c r="K13" s="32" t="str">
+        <f>IF($E13="Nee","NR",IF(ISNUMBER($J13),S13,IF($T13,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M13" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M13" s="31">
+        <v>1</v>
+      </c>
+      <c r="N13" s="10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N13" s="10">
+      <c r="O13" s="10">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O13" s="10">
+        <v>0</v>
+      </c>
+      <c r="P13" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="10">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q13" s="9">
@@ -9219,7 +9219,7 @@
         <v>-I</v>
       </c>
       <c r="T13" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9251,23 +9251,23 @@
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="K14" s="32" t="str">
+        <f>IF($E14="Nee","NR",IF(ISNUMBER($J14),S14,IF($T14,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M14" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M14" s="31">
+        <v>0.99977199999999999</v>
+      </c>
+      <c r="N14" s="10">
         <f t="shared" si="2"/>
         <v>0.99977199999999999</v>
       </c>
-      <c r="N14" s="10">
+      <c r="O14" s="10">
         <f t="shared" si="3"/>
-        <v>0.99977199999999999</v>
-      </c>
-      <c r="O14" s="10">
+        <v>2.2800000000000001E-4</v>
+      </c>
+      <c r="P14" s="10">
         <f t="shared" si="4"/>
-        <v>2.2800000000000001E-4</v>
-      </c>
-      <c r="P14" s="10">
-        <f t="shared" si="5"/>
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="Q14" s="9">
@@ -9283,7 +9283,7 @@
         <v>-I</v>
       </c>
       <c r="T14" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9317,23 +9317,23 @@
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="K15" s="32" t="str">
+        <f>IF($E15="Nee","NR",IF(ISNUMBER($J15),S15,IF($T15,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M15" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M15" s="31">
+        <v>0.99673</v>
+      </c>
+      <c r="N15" s="10">
         <f t="shared" si="2"/>
         <v>0.99673</v>
       </c>
-      <c r="N15" s="10">
+      <c r="O15" s="10">
         <f t="shared" si="3"/>
-        <v>0.99673</v>
-      </c>
-      <c r="O15" s="10">
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="P15" s="10">
         <f t="shared" si="4"/>
-        <v>3.2699999999999999E-3</v>
-      </c>
-      <c r="P15" s="10">
-        <f t="shared" si="5"/>
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="Q15" s="9">
@@ -9349,7 +9349,7 @@
         <v>-I</v>
       </c>
       <c r="T15" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9379,23 +9379,23 @@
         <v>0</v>
       </c>
       <c r="K16" s="32" t="str">
+        <f>IF($E16="Nee","NR",IF(ISNUMBER($J16),S16,IF($T16,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="M16" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M16" s="31">
+        <v>1</v>
+      </c>
+      <c r="N16" s="10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N16" s="10">
+      <c r="O16" s="10">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O16" s="10">
+        <v>0</v>
+      </c>
+      <c r="P16" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="10">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q16" s="9">
@@ -9411,7 +9411,7 @@
         <v>-I</v>
       </c>
       <c r="T16" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9441,23 +9441,23 @@
         <v>0</v>
       </c>
       <c r="K17" s="32" t="str">
+        <f>IF($E17="Nee","NR",IF(ISNUMBER($J17),S17,IF($T17,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="M17" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M17" s="31">
+        <v>1</v>
+      </c>
+      <c r="N17" s="10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N17" s="10">
+      <c r="O17" s="10">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O17" s="10">
+        <v>0</v>
+      </c>
+      <c r="P17" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="10">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q17" s="9">
@@ -9473,7 +9473,7 @@
         <v>-I</v>
       </c>
       <c r="T17" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9505,23 +9505,23 @@
         <v>0</v>
       </c>
       <c r="K18" s="32" t="str">
+        <f>IF($E18="Nee","NR",IF(ISNUMBER($J18),S18,IF($T18,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M18" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M18" s="31">
+        <v>1</v>
+      </c>
+      <c r="N18" s="10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N18" s="10">
+      <c r="O18" s="10">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O18" s="10">
+        <v>0</v>
+      </c>
+      <c r="P18" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="10">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q18" s="9">
@@ -9537,7 +9537,7 @@
         <v>-I</v>
       </c>
       <c r="T18" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9569,23 +9569,23 @@
         <v>-</v>
       </c>
       <c r="K19" s="32" t="str">
+        <f>IF($E19="Nee","NR",IF(ISNUMBER($J19),S19,IF($T19,"D","ND")))</f>
+        <v>D</v>
+      </c>
+      <c r="M19" s="31" t="e">
         <f t="shared" si="1"/>
-        <v>D</v>
-      </c>
-      <c r="M19" s="31" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N19" s="10">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O19" s="10" t="e">
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N19" s="10">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O19" s="10" t="e">
+      <c r="P19" s="10">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P19" s="10">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q19" s="9">
@@ -9601,7 +9601,7 @@
         <v>+0</v>
       </c>
       <c r="T19" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9629,27 +9629,27 @@
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="10">
-        <f t="shared" ref="J20:J22" si="7">IF($E20="Nee",0,IF(H20="Ja",IF(ISNUMBER(I20),I20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
+        <f t="shared" ref="J20:J22" si="6">IF($E20="Nee",0,IF(H20="Ja",IF(ISNUMBER(I20),I20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="K20" s="32" t="str">
+        <f>IF($E20="Nee","NR",IF(ISNUMBER($J20),S20,IF($T20,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M20" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M20" s="31">
+        <v>0.99999800000000005</v>
+      </c>
+      <c r="N20" s="10">
         <f t="shared" si="2"/>
         <v>0.99999800000000005</v>
       </c>
-      <c r="N20" s="10">
+      <c r="O20" s="10">
         <f t="shared" si="3"/>
-        <v>0.99999800000000005</v>
-      </c>
-      <c r="O20" s="10">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="P20" s="10">
         <f t="shared" si="4"/>
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="P20" s="10">
-        <f t="shared" si="5"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="Q20" s="9">
@@ -9665,7 +9665,7 @@
         <v>-I</v>
       </c>
       <c r="T20" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9695,27 +9695,27 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K21" s="32" t="str">
+        <f>IF($E21="Nee","NR",IF(ISNUMBER($J21),S21,IF($T21,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M21" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M21" s="31">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="N21" s="10">
         <f t="shared" si="2"/>
         <v>0.99950000000000006</v>
       </c>
-      <c r="N21" s="10">
+      <c r="O21" s="10">
         <f t="shared" si="3"/>
-        <v>0.99950000000000006</v>
-      </c>
-      <c r="O21" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="P21" s="10">
         <f t="shared" si="4"/>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="P21" s="10">
-        <f t="shared" si="5"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q21" s="9">
@@ -9731,7 +9731,7 @@
         <v>-I</v>
       </c>
       <c r="T21" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9759,27 +9759,27 @@
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="K22" s="32" t="str">
+        <f>IF($E22="Nee","NR",IF(ISNUMBER($J22),S22,IF($T22,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M22" s="31">
         <f t="shared" si="1"/>
-        <v>-I</v>
-      </c>
-      <c r="M22" s="31">
+        <v>0.99999999799999995</v>
+      </c>
+      <c r="N22" s="10">
         <f t="shared" si="2"/>
         <v>0.99999999799999995</v>
       </c>
-      <c r="N22" s="10">
+      <c r="O22" s="10">
         <f t="shared" si="3"/>
-        <v>0.99999999799999995</v>
-      </c>
-      <c r="O22" s="10">
+        <v>2.0000000000000001E-9</v>
+      </c>
+      <c r="P22" s="10">
         <f t="shared" si="4"/>
-        <v>2.0000000000000001E-9</v>
-      </c>
-      <c r="P22" s="10">
-        <f t="shared" si="5"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="Q22" s="9">
@@ -9795,7 +9795,7 @@
         <v>-I</v>
       </c>
       <c r="T22" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10042,7 +10042,7 @@
   <dimension ref="B2:U29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10199,15 +10199,15 @@
         <v>-</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f t="shared" ref="K11:K12" si="1">IF(ISNUMBER($J11),S11,IF($T11,"D","ND"))</f>
+        <f>IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
         <v>ND</v>
       </c>
       <c r="M11" s="31" t="e">
-        <f t="shared" ref="M11:M12" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11:M12" si="1">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N12" si="3">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11:N12" si="2">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10" t="e">
@@ -10263,23 +10263,23 @@
         <v>0</v>
       </c>
       <c r="K12" s="32" t="str">
+        <f>IF($E12="Nee","NR",IF(ISNUMBER($J12),S12,IF($T12,"D","ND")))</f>
+        <v>+III</v>
+      </c>
+      <c r="M12" s="31">
         <f t="shared" si="1"/>
-        <v>+III</v>
-      </c>
-      <c r="M12" s="31">
+        <v>1</v>
+      </c>
+      <c r="N12" s="10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N12" s="10">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
       <c r="O12" s="10">
-        <f t="shared" ref="O12:O13" si="4">IF(AND(F12="Geen faalkans",H12="Nee"),0,J12*$C$3)</f>
+        <f t="shared" ref="O12:O13" si="3">IF(AND(F12="Geen faalkans",H12="Nee"),0,J12*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P13" si="5">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P13" si="4">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
@@ -10295,7 +10295,7 @@
         <v>+III</v>
       </c>
       <c r="T12" s="12" t="b">
-        <f t="shared" ref="T12:T22" si="6">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="5">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -10327,23 +10327,23 @@
         <v>2.4E-2</v>
       </c>
       <c r="K13" s="32" t="str">
-        <f t="shared" ref="K13:K22" si="7">IF(ISNUMBER($J13),S13,IF($T13,"D","ND"))</f>
+        <f>IF($E13="Nee","NR",IF(ISNUMBER($J13),S13,IF($T13,"D","ND")))</f>
         <v>-I</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" ref="M13:M22" si="8">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
+        <f t="shared" ref="M13:M22" si="6">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
         <v>0.97599999999999998</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" ref="N13:N22" si="9">IF(J13="-",1,M13)</f>
+        <f t="shared" ref="N13:N22" si="7">IF(J13="-",1,M13)</f>
         <v>0.97599999999999998</v>
       </c>
       <c r="O13" s="10">
+        <f t="shared" si="3"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="P13" s="10">
         <f t="shared" si="4"/>
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="P13" s="10">
-        <f t="shared" si="5"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="Q13" s="9">
@@ -10359,7 +10359,7 @@
         <v>-I</v>
       </c>
       <c r="T13" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10389,23 +10389,23 @@
         <v>0</v>
       </c>
       <c r="K14" s="32" t="str">
+        <f>IF($E14="Nee","NR",IF(ISNUMBER($J14),S14,IF($T14,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="M14" s="31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N14" s="10">
         <f t="shared" si="7"/>
-        <v>+III</v>
-      </c>
-      <c r="M14" s="31">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N14" s="10">
-        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" ref="O14:O22" si="10">IF(AND(F14="Geen faalkans",H14="Nee"),0,J14*$C$3)</f>
+        <f t="shared" ref="O14:O22" si="8">IF(AND(F14="Geen faalkans",H14="Nee"),0,J14*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" ref="P14:P22" si="11">IF(J14="-",0,O14)</f>
+        <f t="shared" ref="P14:P22" si="9">IF(J14="-",0,O14)</f>
         <v>0</v>
       </c>
       <c r="Q14" s="9">
@@ -10421,7 +10421,7 @@
         <v>+III</v>
       </c>
       <c r="T14" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10451,23 +10451,23 @@
         <v>0</v>
       </c>
       <c r="K15" s="32" t="str">
+        <f>IF($E15="Nee","NR",IF(ISNUMBER($J15),S15,IF($T15,"D","ND")))</f>
+        <v>NR</v>
+      </c>
+      <c r="M15" s="31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N15" s="10">
         <f t="shared" si="7"/>
-        <v>+III</v>
-      </c>
-      <c r="M15" s="31">
+        <v>1</v>
+      </c>
+      <c r="O15" s="10">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N15" s="10">
+        <v>0</v>
+      </c>
+      <c r="P15" s="10">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="O15" s="10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="10">
-        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q15" s="9">
@@ -10483,7 +10483,7 @@
         <v>+III</v>
       </c>
       <c r="T15" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10517,23 +10517,23 @@
         <v>5.9999999999999995E-25</v>
       </c>
       <c r="K16" s="32" t="str">
+        <f>IF($E16="Nee","NR",IF(ISNUMBER($J16),S16,IF($T16,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M16" s="31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N16" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M16" s="31">
+        <v>1</v>
+      </c>
+      <c r="O16" s="10">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N16" s="10">
+        <v>1.1999999999999999E-24</v>
+      </c>
+      <c r="P16" s="10">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="O16" s="10">
-        <f t="shared" si="10"/>
-        <v>1.1999999999999999E-24</v>
-      </c>
-      <c r="P16" s="10">
-        <f t="shared" si="11"/>
         <v>1.1999999999999999E-24</v>
       </c>
       <c r="Q16" s="9">
@@ -10549,7 +10549,7 @@
         <v>-I</v>
       </c>
       <c r="T16" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10583,23 +10583,23 @@
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="K17" s="32" t="str">
+        <f>IF($E17="Nee","NR",IF(ISNUMBER($J17),S17,IF($T17,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M17" s="31">
+        <f t="shared" si="6"/>
+        <v>0.99999300000000002</v>
+      </c>
+      <c r="N17" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M17" s="31">
+        <v>0.99999300000000002</v>
+      </c>
+      <c r="O17" s="10">
         <f t="shared" si="8"/>
-        <v>0.99999300000000002</v>
-      </c>
-      <c r="N17" s="10">
+        <v>1.4E-5</v>
+      </c>
+      <c r="P17" s="10">
         <f t="shared" si="9"/>
-        <v>0.99999300000000002</v>
-      </c>
-      <c r="O17" s="10">
-        <f t="shared" si="10"/>
-        <v>1.4E-5</v>
-      </c>
-      <c r="P17" s="10">
-        <f t="shared" si="11"/>
         <v>1.4E-5</v>
       </c>
       <c r="Q17" s="9">
@@ -10615,7 +10615,7 @@
         <v>-I</v>
       </c>
       <c r="T17" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10649,23 +10649,23 @@
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="K18" s="32" t="str">
+        <f>IF($E18="Nee","NR",IF(ISNUMBER($J18),S18,IF($T18,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M18" s="31">
+        <f t="shared" si="6"/>
+        <v>0.99999800000000005</v>
+      </c>
+      <c r="N18" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M18" s="31">
+        <v>0.99999800000000005</v>
+      </c>
+      <c r="O18" s="10">
         <f t="shared" si="8"/>
-        <v>0.99999800000000005</v>
-      </c>
-      <c r="N18" s="10">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="P18" s="10">
         <f t="shared" si="9"/>
-        <v>0.99999800000000005</v>
-      </c>
-      <c r="O18" s="10">
-        <f t="shared" si="10"/>
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="P18" s="10">
-        <f t="shared" si="11"/>
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="Q18" s="9">
@@ -10681,7 +10681,7 @@
         <v>-I</v>
       </c>
       <c r="T18" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10715,23 +10715,23 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K19" s="32" t="str">
+        <f>IF($E19="Nee","NR",IF(ISNUMBER($J19),S19,IF($T19,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M19" s="31">
+        <f t="shared" si="6"/>
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="N19" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M19" s="31">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="O19" s="10">
         <f t="shared" si="8"/>
-        <v>0.99950000000000006</v>
-      </c>
-      <c r="N19" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="P19" s="10">
         <f t="shared" si="9"/>
-        <v>0.99950000000000006</v>
-      </c>
-      <c r="O19" s="10">
-        <f t="shared" si="10"/>
-        <v>1E-3</v>
-      </c>
-      <c r="P19" s="10">
-        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
       <c r="Q19" s="9">
@@ -10747,7 +10747,7 @@
         <v>-I</v>
       </c>
       <c r="T19" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10779,23 +10779,23 @@
         <v>2.9999999999999998E-15</v>
       </c>
       <c r="K20" s="32" t="str">
+        <f>IF($E20="Nee","NR",IF(ISNUMBER($J20),S20,IF($T20,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M20" s="31">
+        <f t="shared" si="6"/>
+        <v>0.999999999999997</v>
+      </c>
+      <c r="N20" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M20" s="31">
+        <v>0.999999999999997</v>
+      </c>
+      <c r="O20" s="10">
         <f t="shared" si="8"/>
-        <v>0.999999999999997</v>
-      </c>
-      <c r="N20" s="10">
+        <v>5.9999999999999997E-15</v>
+      </c>
+      <c r="P20" s="10">
         <f t="shared" si="9"/>
-        <v>0.999999999999997</v>
-      </c>
-      <c r="O20" s="10">
-        <f t="shared" si="10"/>
-        <v>5.9999999999999997E-15</v>
-      </c>
-      <c r="P20" s="10">
-        <f t="shared" si="11"/>
         <v>5.9999999999999997E-15</v>
       </c>
       <c r="Q20" s="9">
@@ -10811,7 +10811,7 @@
         <v>-I</v>
       </c>
       <c r="T20" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10843,23 +10843,23 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K21" s="32" t="str">
+        <f>IF($E21="Nee","NR",IF(ISNUMBER($J21),S21,IF($T21,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M21" s="31">
+        <f t="shared" si="6"/>
+        <v>0.99995999999999996</v>
+      </c>
+      <c r="N21" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M21" s="31">
+        <v>0.99995999999999996</v>
+      </c>
+      <c r="O21" s="10">
         <f t="shared" si="8"/>
-        <v>0.99995999999999996</v>
-      </c>
-      <c r="N21" s="10">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="P21" s="10">
         <f t="shared" si="9"/>
-        <v>0.99995999999999996</v>
-      </c>
-      <c r="O21" s="10">
-        <f t="shared" si="10"/>
-        <v>8.0000000000000007E-5</v>
-      </c>
-      <c r="P21" s="10">
-        <f t="shared" si="11"/>
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="Q21" s="9">
@@ -10875,7 +10875,7 @@
         <v>-I</v>
       </c>
       <c r="T21" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -10907,23 +10907,23 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="K22" s="32" t="str">
+        <f>IF($E22="Nee","NR",IF(ISNUMBER($J22),S22,IF($T22,"D","ND")))</f>
+        <v>-I</v>
+      </c>
+      <c r="M22" s="31">
+        <f t="shared" si="6"/>
+        <v>0.996</v>
+      </c>
+      <c r="N22" s="10">
         <f t="shared" si="7"/>
-        <v>-I</v>
-      </c>
-      <c r="M22" s="31">
+        <v>0.996</v>
+      </c>
+      <c r="O22" s="10">
         <f t="shared" si="8"/>
-        <v>0.996</v>
-      </c>
-      <c r="N22" s="10">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P22" s="10">
         <f t="shared" si="9"/>
-        <v>0.996</v>
-      </c>
-      <c r="O22" s="10">
-        <f t="shared" si="10"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="P22" s="10">
-        <f t="shared" si="11"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="Q22" s="9">
@@ -10939,7 +10939,7 @@
         <v>-I</v>
       </c>
       <c r="T22" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ASK-41 Fix running the benchmark tests. Still need to fix all remaining errors
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmartktest_traject 16-5.xlsx
+++ b/benchmarktests/testdefinitions/Benchmartktest_traject 16-5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E55E4D2-3BF5-4AD4-A29A-F6628B5D7055}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F892E6B-BCDE-4A30-B91D-46531AF87B87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="10" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="8" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -2208,7 +2208,7 @@
   </sheetPr>
   <dimension ref="B1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
@@ -3406,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="O12" s="32" t="str">
-        <f t="shared" ref="O11:O22" si="6">IF(E12="Nee","NR",IF(ISNUMBER($M12),W12,IF($X12,"D","ND")))</f>
+        <f t="shared" ref="O12:O15" si="6">IF(E12="Nee","NR",IF(ISNUMBER($M12),W12,IF($X12,"D","ND")))</f>
         <v>+III</v>
       </c>
       <c r="Q12" s="31">
@@ -4709,11 +4709,11 @@
         <v>1</v>
       </c>
       <c r="O11" s="30" t="str">
-        <f>IF(E11="Nee","NR",IF(ISNUMBER($M11),W11,IF($X11,"D","ND")))</f>
+        <f t="shared" ref="O11:O22" si="3">IF(E11="Nee","NR",IF(ISNUMBER($M11),W11,IF($X11,"D","ND")))</f>
         <v>+III</v>
       </c>
       <c r="Q11" s="31">
-        <f t="shared" ref="Q11:Q22" si="3">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
+        <f t="shared" ref="Q11:Q22" si="4">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
         <v>1</v>
       </c>
       <c r="R11" s="10">
@@ -4721,7 +4721,7 @@
         <v>1</v>
       </c>
       <c r="S11" s="10">
-        <f t="shared" ref="S11:S22" si="4">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
+        <f t="shared" ref="S11:S22" si="5">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="T11" s="10">
@@ -4785,23 +4785,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O12" s="32" t="str">
-        <f>IF(E12="Nee","NR",IF(ISNUMBER($M12),W12,IF($X12,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>-I</v>
       </c>
       <c r="Q12" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99945015999999998</v>
       </c>
       <c r="R12" s="10">
-        <f t="shared" ref="R12:R22" si="5">IF(M12="-",1,Q12)</f>
+        <f t="shared" ref="R12:R22" si="6">IF(M12="-",1,Q12)</f>
         <v>0.99945015999999998</v>
       </c>
       <c r="S12" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5076E-3</v>
       </c>
       <c r="T12" s="10">
-        <f t="shared" ref="T12:T22" si="6">IF(L12="-",0,S12)</f>
+        <f t="shared" ref="T12:T22" si="7">IF(L12="-",0,S12)</f>
         <v>3.5076E-3</v>
       </c>
       <c r="U12" s="9">
@@ -4817,7 +4817,7 @@
         <v>-I</v>
       </c>
       <c r="X12" s="12" t="b">
-        <f t="shared" ref="X12:X22" si="7">IF($E12="Ja",IF($I12="Ja",NOT(ISNUMBER($J12)),FALSE),FALSE)</f>
+        <f t="shared" ref="X12:X22" si="8">IF($E12="Ja",IF($I12="Ja",NOT(ISNUMBER($J12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -4861,23 +4861,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O13" s="32" t="str">
-        <f>IF(E13="Nee","NR",IF(ISNUMBER($M13),W13,IF($X13,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>-I</v>
       </c>
       <c r="Q13" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R13" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="S13" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S13" s="10">
-        <f t="shared" si="4"/>
         <v>1.48E-49</v>
       </c>
       <c r="T13" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.48E-49</v>
       </c>
       <c r="U13" s="9">
@@ -4893,7 +4893,7 @@
         <v>-I</v>
       </c>
       <c r="X13" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4933,23 +4933,23 @@
         <v>1</v>
       </c>
       <c r="O14" s="32" t="str">
-        <f>IF(E14="Nee","NR",IF(ISNUMBER($M14),W14,IF($X14,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>NR</v>
       </c>
       <c r="Q14" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R14" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="S14" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S14" s="10">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U14" s="9">
@@ -4965,7 +4965,7 @@
         <v>+III</v>
       </c>
       <c r="X14" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5009,23 +5009,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O15" s="32" t="str">
-        <f>IF(E15="Nee","NR",IF(ISNUMBER($M15),W15,IF($X15,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>-I</v>
       </c>
       <c r="Q15" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99944895359999997</v>
       </c>
       <c r="R15" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99944895359999997</v>
+      </c>
+      <c r="S15" s="10">
         <f t="shared" si="5"/>
-        <v>0.99944895359999997</v>
-      </c>
-      <c r="S15" s="10">
-        <f t="shared" si="4"/>
         <v>3.5152960000000002E-3</v>
       </c>
       <c r="T15" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.5152960000000002E-3</v>
       </c>
       <c r="U15" s="9">
@@ -5041,7 +5041,7 @@
         <v>-I</v>
       </c>
       <c r="X15" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5081,23 +5081,23 @@
         <v>1</v>
       </c>
       <c r="O16" s="32" t="str">
-        <f>IF(E16="Nee","NR",IF(ISNUMBER($M16),W16,IF($X16,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>NR</v>
       </c>
       <c r="Q16" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R16" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="S16" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S16" s="10">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T16" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U16" s="9">
@@ -5113,7 +5113,7 @@
         <v>+III</v>
       </c>
       <c r="X16" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5162,23 +5162,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O17" s="32" t="str">
-        <f>IF(E17="Nee","NR",IF(ISNUMBER($M17),W17,IF($X17,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>-I</v>
       </c>
       <c r="Q17" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9999768</v>
       </c>
       <c r="R17" s="10">
+        <f t="shared" si="6"/>
+        <v>0.9999768</v>
+      </c>
+      <c r="S17" s="10">
         <f t="shared" si="5"/>
-        <v>0.9999768</v>
-      </c>
-      <c r="S17" s="10">
-        <f t="shared" si="4"/>
         <v>1.4800000000000002E-4</v>
       </c>
       <c r="T17" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.4800000000000002E-4</v>
       </c>
       <c r="U17" s="9">
@@ -5194,7 +5194,7 @@
         <v>-I</v>
       </c>
       <c r="X17" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5218,7 +5218,7 @@
         <v>2.3800000000000001E-4</v>
       </c>
       <c r="H18" s="26">
-        <f t="shared" ref="H18:H22" si="8">G18*2.32</f>
+        <f t="shared" ref="H18:H22" si="9">G18*2.32</f>
         <v>5.5216E-4</v>
       </c>
       <c r="I18" s="8" t="s">
@@ -5243,23 +5243,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O18" s="32" t="str">
-        <f>IF(E18="Nee","NR",IF(ISNUMBER($M18),W18,IF($X18,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>-I</v>
       </c>
       <c r="Q18" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99999999976800003</v>
       </c>
       <c r="R18" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99999999976800003</v>
+      </c>
+      <c r="S18" s="10">
         <f t="shared" si="5"/>
-        <v>0.99999999976800003</v>
-      </c>
-      <c r="S18" s="10">
-        <f t="shared" si="4"/>
         <v>1.4800000000000001E-9</v>
       </c>
       <c r="T18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.4800000000000001E-9</v>
       </c>
       <c r="U18" s="9">
@@ -5275,7 +5275,7 @@
         <v>-I</v>
       </c>
       <c r="X18" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5319,23 +5319,23 @@
         <v>-</v>
       </c>
       <c r="O19" s="32" t="str">
-        <f>IF(E19="Nee","NR",IF(ISNUMBER($M19),W19,IF($X19,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>D</v>
       </c>
       <c r="Q19" s="31" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R19" s="10">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S19" s="10" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="R19" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="S19" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="T19" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U19" s="9">
@@ -5351,7 +5351,7 @@
         <v>+III</v>
       </c>
       <c r="X19" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -5387,11 +5387,11 @@
         <v>0</v>
       </c>
       <c r="L20" s="31">
-        <f t="shared" ref="L20:L22" si="9">IF($E20="Nee",0,IF(I20="Ja",IF(ISNUMBER(J20),J20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
+        <f t="shared" ref="L20:L22" si="10">IF($E20="Nee",0,IF(I20="Ja",IF(ISNUMBER(J20),J20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
         <v>0</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" ref="M20:M22" si="10">IF($E20="Nee",0,IF(I20="Ja",IF(ISNUMBER(K20),K20,"-"),IF(ISNUMBER(H20),H20,"-")))</f>
+        <f t="shared" ref="M20:M22" si="11">IF($E20="Nee",0,IF(I20="Ja",IF(ISNUMBER(K20),K20,"-"),IF(ISNUMBER(H20),H20,"-")))</f>
         <v>0</v>
       </c>
       <c r="N20" s="11">
@@ -5399,23 +5399,23 @@
         <v>1</v>
       </c>
       <c r="O20" s="32" t="str">
-        <f>IF(E20="Nee","NR",IF(ISNUMBER($M20),W20,IF($X20,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>+III</v>
       </c>
       <c r="Q20" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R20" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="S20" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S20" s="10">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U20" s="9">
@@ -5431,7 +5431,7 @@
         <v>+III</v>
       </c>
       <c r="X20" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5455,7 +5455,7 @@
         <v>0.1</v>
       </c>
       <c r="H21" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.23199999999999998</v>
       </c>
       <c r="I21" s="8" t="s">
@@ -5468,11 +5468,11 @@
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="L21" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1E-8</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="N21" s="11">
@@ -5480,23 +5480,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O21" s="32" t="str">
-        <f>IF(E21="Nee","NR",IF(ISNUMBER($M21),W21,IF($X21,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>-I</v>
       </c>
       <c r="Q21" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99999997679999997</v>
       </c>
       <c r="R21" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="S21" s="10">
         <f t="shared" si="5"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="S21" s="10">
-        <f t="shared" si="4"/>
         <v>1.48E-7</v>
       </c>
       <c r="T21" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.48E-7</v>
       </c>
       <c r="U21" s="9">
@@ -5512,7 +5512,7 @@
         <v>-I</v>
       </c>
       <c r="X21" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5536,7 +5536,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="H22" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.22968</v>
       </c>
       <c r="I22" s="8" t="s">
@@ -5549,11 +5549,11 @@
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="L22" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1E-8</v>
       </c>
       <c r="M22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="N22" s="11">
@@ -5561,23 +5561,23 @@
         <v>2.3200000000000003</v>
       </c>
       <c r="O22" s="32" t="str">
-        <f>IF(E22="Nee","NR",IF(ISNUMBER($M22),W22,IF($X22,"D","ND")))</f>
+        <f t="shared" si="3"/>
         <v>-I</v>
       </c>
       <c r="Q22" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99999997679999997</v>
       </c>
       <c r="R22" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="S22" s="10">
         <f t="shared" si="5"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="S22" s="10">
-        <f t="shared" si="4"/>
         <v>1.48E-7</v>
       </c>
       <c r="T22" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.48E-7</v>
       </c>
       <c r="U22" s="9">
@@ -5593,7 +5593,7 @@
         <v>-I</v>
       </c>
       <c r="X22" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -7428,7 +7428,7 @@
   <dimension ref="B2:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7568,7 +7568,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="43">
-        <v>20.93</v>
+        <v>24</v>
       </c>
       <c r="E11" s="44" t="s">
         <v>21</v>
@@ -7907,19 +7907,19 @@
         <v>-</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f>IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
+        <f t="shared" ref="K11:K22" si="1">IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
         <v>ND</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" ref="M11:M12" si="1">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11:M12" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>1</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N12" si="2">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11:N12" si="3">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11:O12" si="3">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
+        <f t="shared" ref="O11:O12" si="4">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P11" s="10">
@@ -7973,23 +7973,23 @@
         <v>0</v>
       </c>
       <c r="K12" s="32" t="str">
-        <f>IF($E12="Nee","NR",IF(ISNUMBER($J12),S12,IF($T12,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M12" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P13" si="4">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P13" si="5">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
@@ -8005,7 +8005,7 @@
         <v>+III</v>
       </c>
       <c r="T12" s="12" t="b">
-        <f t="shared" ref="T12:T22" si="5">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="6">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -8039,23 +8039,23 @@
         <v>5.9999999999999997E-7</v>
       </c>
       <c r="K13" s="32" t="str">
-        <f>IF($E13="Nee","NR",IF(ISNUMBER($J13),S13,IF($T13,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" ref="M13:M22" si="6">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
+        <f t="shared" ref="M13:M22" si="7">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
         <v>0.99999939999999998</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" ref="N13:N22" si="7">IF(J13="-",1,M13)</f>
+        <f t="shared" ref="N13:N22" si="8">IF(J13="-",1,M13)</f>
         <v>0.99999939999999998</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" ref="O13:O22" si="8">IF(AND(F13="Geen faalkans",H13="Nee"),0,J13*$C$3)</f>
+        <f t="shared" ref="O13:O22" si="9">IF(AND(F13="Geen faalkans",H13="Nee"),0,J13*$C$3)</f>
         <v>1.7999999999999999E-6</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.7999999999999999E-6</v>
       </c>
       <c r="Q13" s="9">
@@ -8071,7 +8071,7 @@
         <v>-I</v>
       </c>
       <c r="T13" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8103,23 +8103,23 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="K14" s="32" t="str">
-        <f>IF($E14="Nee","NR",IF(ISNUMBER($J14),S14,IF($T14,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M14" s="31">
-        <f t="shared" si="6"/>
-        <v>0.99999499999999997</v>
-      </c>
-      <c r="N14" s="10">
         <f t="shared" si="7"/>
         <v>0.99999499999999997</v>
       </c>
+      <c r="N14" s="10">
+        <f t="shared" si="8"/>
+        <v>0.99999499999999997</v>
+      </c>
       <c r="O14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" ref="P14:P22" si="9">IF(J14="-",0,O14)</f>
+        <f t="shared" ref="P14:P22" si="10">IF(J14="-",0,O14)</f>
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="Q14" s="9">
@@ -8135,7 +8135,7 @@
         <v>-I</v>
       </c>
       <c r="T14" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8169,23 +8169,23 @@
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="K15" s="32" t="str">
-        <f>IF($E15="Nee","NR",IF(ISNUMBER($J15),S15,IF($T15,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M15" s="31">
-        <f t="shared" si="6"/>
-        <v>0.999999992</v>
-      </c>
-      <c r="N15" s="10">
         <f t="shared" si="7"/>
         <v>0.999999992</v>
       </c>
+      <c r="N15" s="10">
+        <f t="shared" si="8"/>
+        <v>0.999999992</v>
+      </c>
       <c r="O15" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.4000000000000003E-8</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.4000000000000003E-8</v>
       </c>
       <c r="Q15" s="9">
@@ -8201,7 +8201,7 @@
         <v>-I</v>
       </c>
       <c r="T15" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8235,23 +8235,23 @@
         <v>0</v>
       </c>
       <c r="K16" s="32" t="str">
-        <f>IF($E16="Nee","NR",IF(ISNUMBER($J16),S16,IF($T16,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M16" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q16" s="9">
@@ -8267,7 +8267,7 @@
         <v>+III</v>
       </c>
       <c r="T16" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8301,23 +8301,23 @@
         <v>2.546E-5</v>
       </c>
       <c r="K17" s="32" t="str">
-        <f>IF($E17="Nee","NR",IF(ISNUMBER($J17),S17,IF($T17,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M17" s="31">
-        <f t="shared" si="6"/>
-        <v>0.99997453999999997</v>
-      </c>
-      <c r="N17" s="10">
         <f t="shared" si="7"/>
         <v>0.99997453999999997</v>
       </c>
+      <c r="N17" s="10">
+        <f t="shared" si="8"/>
+        <v>0.99997453999999997</v>
+      </c>
       <c r="O17" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.6379999999999997E-5</v>
       </c>
       <c r="P17" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.6379999999999997E-5</v>
       </c>
       <c r="Q17" s="9">
@@ -8333,7 +8333,7 @@
         <v>-I</v>
       </c>
       <c r="T17" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8365,23 +8365,23 @@
         <v>6.6600000000000003E-4</v>
       </c>
       <c r="K18" s="32" t="str">
-        <f>IF($E18="Nee","NR",IF(ISNUMBER($J18),S18,IF($T18,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M18" s="31">
-        <f t="shared" si="6"/>
-        <v>0.99933399999999994</v>
-      </c>
-      <c r="N18" s="10">
         <f t="shared" si="7"/>
         <v>0.99933399999999994</v>
       </c>
+      <c r="N18" s="10">
+        <f t="shared" si="8"/>
+        <v>0.99933399999999994</v>
+      </c>
       <c r="O18" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.9980000000000002E-3</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.9980000000000002E-3</v>
       </c>
       <c r="Q18" s="9">
@@ -8397,7 +8397,7 @@
         <v>-I</v>
       </c>
       <c r="T18" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8431,23 +8431,23 @@
         <v>1.2999999999999999E-3</v>
       </c>
       <c r="K19" s="32" t="str">
-        <f>IF($E19="Nee","NR",IF(ISNUMBER($J19),S19,IF($T19,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M19" s="31">
-        <f t="shared" si="6"/>
-        <v>0.99870000000000003</v>
-      </c>
-      <c r="N19" s="10">
         <f t="shared" si="7"/>
         <v>0.99870000000000003</v>
       </c>
+      <c r="N19" s="10">
+        <f t="shared" si="8"/>
+        <v>0.99870000000000003</v>
+      </c>
       <c r="O19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="Q19" s="9">
@@ -8463,7 +8463,7 @@
         <v>-I</v>
       </c>
       <c r="T19" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8495,23 +8495,23 @@
         <v>0</v>
       </c>
       <c r="K20" s="32" t="str">
-        <f>IF($E20="Nee","NR",IF(ISNUMBER($J20),S20,IF($T20,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M20" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q20" s="9">
@@ -8527,7 +8527,7 @@
         <v>+III</v>
       </c>
       <c r="T20" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8561,23 +8561,23 @@
         <v>0</v>
       </c>
       <c r="K21" s="32" t="str">
-        <f>IF($E21="Nee","NR",IF(ISNUMBER($J21),S21,IF($T21,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M21" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q21" s="9">
@@ -8593,7 +8593,7 @@
         <v>+III</v>
       </c>
       <c r="T21" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8623,23 +8623,23 @@
         <v>0</v>
       </c>
       <c r="K22" s="32" t="str">
-        <f>IF($E22="Nee","NR",IF(ISNUMBER($J22),S22,IF($T22,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>NR</v>
       </c>
       <c r="M22" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q22" s="9">
@@ -8655,7 +8655,7 @@
         <v>+III</v>
       </c>
       <c r="T22" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9059,19 +9059,19 @@
         <v>0</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f>IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
+        <f t="shared" ref="K11:K22" si="1">IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
         <v>NR</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" ref="M11:M22" si="1">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11:M22" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>1</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N22" si="2">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11:N22" si="3">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11:O22" si="3">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
+        <f t="shared" ref="O11:O22" si="4">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P11" s="10">
@@ -9121,23 +9121,23 @@
         <v>-</v>
       </c>
       <c r="K12" s="32" t="str">
-        <f>IF($E12="Nee","NR",IF(ISNUMBER($J12),S12,IF($T12,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>ND</v>
       </c>
       <c r="M12" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P22" si="4">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P22" si="5">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
@@ -9153,7 +9153,7 @@
         <v>+0</v>
       </c>
       <c r="T12" s="12" t="b">
-        <f t="shared" ref="T12:T22" si="5">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="6">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -9187,23 +9187,23 @@
         <v>0</v>
       </c>
       <c r="K13" s="32" t="str">
-        <f>IF($E13="Nee","NR",IF(ISNUMBER($J13),S13,IF($T13,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q13" s="9">
@@ -9219,7 +9219,7 @@
         <v>-I</v>
       </c>
       <c r="T13" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9251,23 +9251,23 @@
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="K14" s="32" t="str">
-        <f>IF($E14="Nee","NR",IF(ISNUMBER($J14),S14,IF($T14,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M14" s="31">
-        <f t="shared" si="1"/>
-        <v>0.99977199999999999</v>
-      </c>
-      <c r="N14" s="10">
         <f t="shared" si="2"/>
         <v>0.99977199999999999</v>
       </c>
+      <c r="N14" s="10">
+        <f t="shared" si="3"/>
+        <v>0.99977199999999999</v>
+      </c>
       <c r="O14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="Q14" s="9">
@@ -9283,7 +9283,7 @@
         <v>-I</v>
       </c>
       <c r="T14" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9317,23 +9317,23 @@
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="K15" s="32" t="str">
-        <f>IF($E15="Nee","NR",IF(ISNUMBER($J15),S15,IF($T15,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M15" s="31">
-        <f t="shared" si="1"/>
-        <v>0.99673</v>
-      </c>
-      <c r="N15" s="10">
         <f t="shared" si="2"/>
         <v>0.99673</v>
       </c>
+      <c r="N15" s="10">
+        <f t="shared" si="3"/>
+        <v>0.99673</v>
+      </c>
       <c r="O15" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="Q15" s="9">
@@ -9349,7 +9349,7 @@
         <v>-I</v>
       </c>
       <c r="T15" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9379,23 +9379,23 @@
         <v>0</v>
       </c>
       <c r="K16" s="32" t="str">
-        <f>IF($E16="Nee","NR",IF(ISNUMBER($J16),S16,IF($T16,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>NR</v>
       </c>
       <c r="M16" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q16" s="9">
@@ -9411,7 +9411,7 @@
         <v>-I</v>
       </c>
       <c r="T16" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9441,23 +9441,23 @@
         <v>0</v>
       </c>
       <c r="K17" s="32" t="str">
-        <f>IF($E17="Nee","NR",IF(ISNUMBER($J17),S17,IF($T17,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>NR</v>
       </c>
       <c r="M17" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N17" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P17" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q17" s="9">
@@ -9473,7 +9473,7 @@
         <v>-I</v>
       </c>
       <c r="T17" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9505,23 +9505,23 @@
         <v>0</v>
       </c>
       <c r="K18" s="32" t="str">
-        <f>IF($E18="Nee","NR",IF(ISNUMBER($J18),S18,IF($T18,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M18" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q18" s="9">
@@ -9537,7 +9537,7 @@
         <v>-I</v>
       </c>
       <c r="T18" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9569,23 +9569,23 @@
         <v>-</v>
       </c>
       <c r="K19" s="32" t="str">
-        <f>IF($E19="Nee","NR",IF(ISNUMBER($J19),S19,IF($T19,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>D</v>
       </c>
       <c r="M19" s="31" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O19" s="10" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q19" s="9">
@@ -9601,7 +9601,7 @@
         <v>+0</v>
       </c>
       <c r="T19" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -9629,27 +9629,27 @@
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="10">
-        <f t="shared" ref="J20:J22" si="6">IF($E20="Nee",0,IF(H20="Ja",IF(ISNUMBER(I20),I20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
+        <f t="shared" ref="J20:J22" si="7">IF($E20="Nee",0,IF(H20="Ja",IF(ISNUMBER(I20),I20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="K20" s="32" t="str">
-        <f>IF($E20="Nee","NR",IF(ISNUMBER($J20),S20,IF($T20,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M20" s="31">
-        <f t="shared" si="1"/>
-        <v>0.99999800000000005</v>
-      </c>
-      <c r="N20" s="10">
         <f t="shared" si="2"/>
         <v>0.99999800000000005</v>
       </c>
+      <c r="N20" s="10">
+        <f t="shared" si="3"/>
+        <v>0.99999800000000005</v>
+      </c>
       <c r="O20" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="Q20" s="9">
@@ -9665,7 +9665,7 @@
         <v>-I</v>
       </c>
       <c r="T20" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9695,27 +9695,27 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K21" s="32" t="str">
-        <f>IF($E21="Nee","NR",IF(ISNUMBER($J21),S21,IF($T21,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M21" s="31">
-        <f t="shared" si="1"/>
-        <v>0.99950000000000006</v>
-      </c>
-      <c r="N21" s="10">
         <f t="shared" si="2"/>
         <v>0.99950000000000006</v>
       </c>
+      <c r="N21" s="10">
+        <f t="shared" si="3"/>
+        <v>0.99950000000000006</v>
+      </c>
       <c r="O21" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q21" s="9">
@@ -9731,7 +9731,7 @@
         <v>-I</v>
       </c>
       <c r="T21" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9759,27 +9759,27 @@
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="K22" s="32" t="str">
-        <f>IF($E22="Nee","NR",IF(ISNUMBER($J22),S22,IF($T22,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M22" s="31">
-        <f t="shared" si="1"/>
-        <v>0.99999999799999995</v>
-      </c>
-      <c r="N22" s="10">
         <f t="shared" si="2"/>
         <v>0.99999999799999995</v>
       </c>
+      <c r="N22" s="10">
+        <f t="shared" si="3"/>
+        <v>0.99999999799999995</v>
+      </c>
       <c r="O22" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="Q22" s="9">
@@ -9795,7 +9795,7 @@
         <v>-I</v>
       </c>
       <c r="T22" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10041,7 +10041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A27DBF-2298-4509-84AE-DCEFED147711}">
   <dimension ref="B2:U29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -10199,15 +10199,15 @@
         <v>-</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f>IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
+        <f t="shared" ref="K11:K22" si="1">IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
         <v>ND</v>
       </c>
       <c r="M11" s="31" t="e">
-        <f t="shared" ref="M11:M12" si="1">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11:M12" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N12" si="2">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11:N12" si="3">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10" t="e">
@@ -10263,23 +10263,23 @@
         <v>0</v>
       </c>
       <c r="K12" s="32" t="str">
-        <f>IF($E12="Nee","NR",IF(ISNUMBER($J12),S12,IF($T12,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M12" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" ref="O12:O13" si="3">IF(AND(F12="Geen faalkans",H12="Nee"),0,J12*$C$3)</f>
+        <f t="shared" ref="O12:O13" si="4">IF(AND(F12="Geen faalkans",H12="Nee"),0,J12*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P13" si="4">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P13" si="5">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
@@ -10295,7 +10295,7 @@
         <v>+III</v>
       </c>
       <c r="T12" s="12" t="b">
-        <f t="shared" ref="T12:T22" si="5">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="6">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -10327,23 +10327,23 @@
         <v>2.4E-2</v>
       </c>
       <c r="K13" s="32" t="str">
-        <f>IF($E13="Nee","NR",IF(ISNUMBER($J13),S13,IF($T13,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" ref="M13:M22" si="6">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
+        <f t="shared" ref="M13:M22" si="7">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
         <v>0.97599999999999998</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" ref="N13:N22" si="7">IF(J13="-",1,M13)</f>
+        <f t="shared" ref="N13:N22" si="8">IF(J13="-",1,M13)</f>
         <v>0.97599999999999998</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="Q13" s="9">
@@ -10359,7 +10359,7 @@
         <v>-I</v>
       </c>
       <c r="T13" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10389,23 +10389,23 @@
         <v>0</v>
       </c>
       <c r="K14" s="32" t="str">
-        <f>IF($E14="Nee","NR",IF(ISNUMBER($J14),S14,IF($T14,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>NR</v>
       </c>
       <c r="M14" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" ref="O14:O22" si="8">IF(AND(F14="Geen faalkans",H14="Nee"),0,J14*$C$3)</f>
+        <f t="shared" ref="O14:O22" si="9">IF(AND(F14="Geen faalkans",H14="Nee"),0,J14*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" ref="P14:P22" si="9">IF(J14="-",0,O14)</f>
+        <f t="shared" ref="P14:P22" si="10">IF(J14="-",0,O14)</f>
         <v>0</v>
       </c>
       <c r="Q14" s="9">
@@ -10421,7 +10421,7 @@
         <v>+III</v>
       </c>
       <c r="T14" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10451,23 +10451,23 @@
         <v>0</v>
       </c>
       <c r="K15" s="32" t="str">
-        <f>IF($E15="Nee","NR",IF(ISNUMBER($J15),S15,IF($T15,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>NR</v>
       </c>
       <c r="M15" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q15" s="9">
@@ -10483,7 +10483,7 @@
         <v>+III</v>
       </c>
       <c r="T15" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10517,23 +10517,23 @@
         <v>5.9999999999999995E-25</v>
       </c>
       <c r="K16" s="32" t="str">
-        <f>IF($E16="Nee","NR",IF(ISNUMBER($J16),S16,IF($T16,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M16" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1999999999999999E-24</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1999999999999999E-24</v>
       </c>
       <c r="Q16" s="9">
@@ -10549,7 +10549,7 @@
         <v>-I</v>
       </c>
       <c r="T16" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10583,23 +10583,23 @@
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="K17" s="32" t="str">
-        <f>IF($E17="Nee","NR",IF(ISNUMBER($J17),S17,IF($T17,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M17" s="31">
-        <f t="shared" si="6"/>
-        <v>0.99999300000000002</v>
-      </c>
-      <c r="N17" s="10">
         <f t="shared" si="7"/>
         <v>0.99999300000000002</v>
       </c>
+      <c r="N17" s="10">
+        <f t="shared" si="8"/>
+        <v>0.99999300000000002</v>
+      </c>
       <c r="O17" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.4E-5</v>
       </c>
       <c r="P17" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.4E-5</v>
       </c>
       <c r="Q17" s="9">
@@ -10615,7 +10615,7 @@
         <v>-I</v>
       </c>
       <c r="T17" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10649,23 +10649,23 @@
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="K18" s="32" t="str">
-        <f>IF($E18="Nee","NR",IF(ISNUMBER($J18),S18,IF($T18,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M18" s="31">
-        <f t="shared" si="6"/>
-        <v>0.99999800000000005</v>
-      </c>
-      <c r="N18" s="10">
         <f t="shared" si="7"/>
         <v>0.99999800000000005</v>
       </c>
+      <c r="N18" s="10">
+        <f t="shared" si="8"/>
+        <v>0.99999800000000005</v>
+      </c>
       <c r="O18" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="Q18" s="9">
@@ -10681,7 +10681,7 @@
         <v>-I</v>
       </c>
       <c r="T18" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10715,23 +10715,23 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K19" s="32" t="str">
-        <f>IF($E19="Nee","NR",IF(ISNUMBER($J19),S19,IF($T19,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M19" s="31">
-        <f t="shared" si="6"/>
-        <v>0.99950000000000006</v>
-      </c>
-      <c r="N19" s="10">
         <f t="shared" si="7"/>
         <v>0.99950000000000006</v>
       </c>
+      <c r="N19" s="10">
+        <f t="shared" si="8"/>
+        <v>0.99950000000000006</v>
+      </c>
       <c r="O19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1E-3</v>
       </c>
       <c r="Q19" s="9">
@@ -10747,7 +10747,7 @@
         <v>-I</v>
       </c>
       <c r="T19" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10779,23 +10779,23 @@
         <v>2.9999999999999998E-15</v>
       </c>
       <c r="K20" s="32" t="str">
-        <f>IF($E20="Nee","NR",IF(ISNUMBER($J20),S20,IF($T20,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M20" s="31">
-        <f t="shared" si="6"/>
-        <v>0.999999999999997</v>
-      </c>
-      <c r="N20" s="10">
         <f t="shared" si="7"/>
         <v>0.999999999999997</v>
       </c>
+      <c r="N20" s="10">
+        <f t="shared" si="8"/>
+        <v>0.999999999999997</v>
+      </c>
       <c r="O20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9999999999999997E-15</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.9999999999999997E-15</v>
       </c>
       <c r="Q20" s="9">
@@ -10811,7 +10811,7 @@
         <v>-I</v>
       </c>
       <c r="T20" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10843,23 +10843,23 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K21" s="32" t="str">
-        <f>IF($E21="Nee","NR",IF(ISNUMBER($J21),S21,IF($T21,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M21" s="31">
-        <f t="shared" si="6"/>
-        <v>0.99995999999999996</v>
-      </c>
-      <c r="N21" s="10">
         <f t="shared" si="7"/>
         <v>0.99995999999999996</v>
       </c>
+      <c r="N21" s="10">
+        <f t="shared" si="8"/>
+        <v>0.99995999999999996</v>
+      </c>
       <c r="O21" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="Q21" s="9">
@@ -10875,7 +10875,7 @@
         <v>-I</v>
       </c>
       <c r="T21" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10907,23 +10907,23 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="K22" s="32" t="str">
-        <f>IF($E22="Nee","NR",IF(ISNUMBER($J22),S22,IF($T22,"D","ND")))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M22" s="31">
-        <f t="shared" si="6"/>
-        <v>0.996</v>
-      </c>
-      <c r="N22" s="10">
         <f t="shared" si="7"/>
         <v>0.996</v>
       </c>
+      <c r="N22" s="10">
+        <f t="shared" si="8"/>
+        <v>0.996</v>
+      </c>
       <c r="O22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="Q22" s="9">
@@ -10939,7 +10939,7 @@
         <v>-I</v>
       </c>
       <c r="T22" s="12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>